<commit_message>
update modules and data file
</commit_message>
<xml_diff>
--- a/data/us_sales_update.xlsx
+++ b/data/us_sales_update.xlsx
@@ -19,8 +19,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
-    <numFmt numFmtId="166" formatCode="yyyy-mm-dd h:mm:ss"/>
-    <numFmt numFmtId="167" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="166" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="167" formatCode="yyyy-mm-dd h:mm:ss"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -114,7 +114,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -142,12 +142,15 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -546,256 +549,256 @@
           <t>Brand</t>
         </is>
       </c>
-      <c r="C1" s="9" t="n">
+      <c r="C1" s="12" t="n">
         <v>43466</v>
       </c>
-      <c r="D1" s="9" t="n">
+      <c r="D1" s="12" t="n">
         <v>43497</v>
       </c>
-      <c r="E1" s="9" t="n">
+      <c r="E1" s="12" t="n">
         <v>43525</v>
       </c>
-      <c r="F1" s="9" t="n">
+      <c r="F1" s="12" t="n">
         <v>43556</v>
       </c>
-      <c r="G1" s="9" t="n">
+      <c r="G1" s="12" t="n">
         <v>43586</v>
       </c>
-      <c r="H1" s="9" t="n">
+      <c r="H1" s="12" t="n">
         <v>43617</v>
       </c>
-      <c r="I1" s="9" t="n">
+      <c r="I1" s="12" t="n">
         <v>43647</v>
       </c>
-      <c r="J1" s="9" t="n">
+      <c r="J1" s="12" t="n">
         <v>43678</v>
       </c>
-      <c r="K1" s="9" t="n">
+      <c r="K1" s="12" t="n">
         <v>43709</v>
       </c>
-      <c r="L1" s="9" t="n">
+      <c r="L1" s="12" t="n">
         <v>43739</v>
       </c>
-      <c r="M1" s="9" t="n">
+      <c r="M1" s="12" t="n">
         <v>43770</v>
       </c>
-      <c r="N1" s="9" t="n">
+      <c r="N1" s="12" t="n">
         <v>43800</v>
       </c>
-      <c r="O1" s="9" t="n">
+      <c r="O1" s="12" t="n">
         <v>43831</v>
       </c>
-      <c r="P1" s="9" t="n">
+      <c r="P1" s="12" t="n">
         <v>43862</v>
       </c>
-      <c r="Q1" s="9" t="n">
+      <c r="Q1" s="12" t="n">
         <v>43891</v>
       </c>
-      <c r="R1" s="9" t="n">
+      <c r="R1" s="12" t="n">
         <v>43922</v>
       </c>
-      <c r="S1" s="9" t="n">
+      <c r="S1" s="12" t="n">
         <v>43952</v>
       </c>
-      <c r="T1" s="9" t="n">
+      <c r="T1" s="12" t="n">
         <v>43983</v>
       </c>
-      <c r="U1" s="9" t="n">
+      <c r="U1" s="12" t="n">
         <v>44013</v>
       </c>
-      <c r="V1" s="9" t="n">
+      <c r="V1" s="12" t="n">
         <v>44044</v>
       </c>
-      <c r="W1" s="9" t="n">
+      <c r="W1" s="12" t="n">
         <v>44075</v>
       </c>
-      <c r="X1" s="9" t="n">
+      <c r="X1" s="12" t="n">
         <v>44105</v>
       </c>
-      <c r="Y1" s="9" t="n">
+      <c r="Y1" s="12" t="n">
         <v>44136</v>
       </c>
-      <c r="Z1" s="9" t="n">
+      <c r="Z1" s="12" t="n">
         <v>44166</v>
       </c>
-      <c r="AA1" s="9" t="n">
+      <c r="AA1" s="12" t="n">
         <v>44197</v>
       </c>
-      <c r="AB1" s="9" t="n">
+      <c r="AB1" s="12" t="n">
         <v>44228</v>
       </c>
-      <c r="AC1" s="9" t="n">
+      <c r="AC1" s="12" t="n">
         <v>44256</v>
       </c>
-      <c r="AD1" s="9" t="n">
+      <c r="AD1" s="12" t="n">
         <v>44287</v>
       </c>
-      <c r="AE1" s="9" t="n">
+      <c r="AE1" s="12" t="n">
         <v>44317</v>
       </c>
-      <c r="AF1" s="9" t="n">
+      <c r="AF1" s="12" t="n">
         <v>44348</v>
       </c>
-      <c r="AG1" s="9" t="n">
+      <c r="AG1" s="12" t="n">
         <v>44378</v>
       </c>
-      <c r="AH1" s="9" t="n">
+      <c r="AH1" s="12" t="n">
         <v>44409</v>
       </c>
-      <c r="AI1" s="9" t="n">
+      <c r="AI1" s="12" t="n">
         <v>44440</v>
       </c>
-      <c r="AJ1" s="9" t="n">
+      <c r="AJ1" s="12" t="n">
         <v>44470</v>
       </c>
-      <c r="AK1" s="9" t="n">
+      <c r="AK1" s="12" t="n">
         <v>44501</v>
       </c>
-      <c r="AL1" s="9" t="n">
+      <c r="AL1" s="12" t="n">
         <v>44531</v>
       </c>
-      <c r="AM1" s="9" t="n">
+      <c r="AM1" s="12" t="n">
         <v>44562</v>
       </c>
-      <c r="AN1" s="9" t="n">
+      <c r="AN1" s="12" t="n">
         <v>44593</v>
       </c>
-      <c r="AO1" s="9" t="n">
+      <c r="AO1" s="12" t="n">
         <v>44621</v>
       </c>
-      <c r="AP1" s="9" t="n">
+      <c r="AP1" s="12" t="n">
         <v>44652</v>
       </c>
-      <c r="AQ1" s="9" t="n">
+      <c r="AQ1" s="12" t="n">
         <v>44682</v>
       </c>
-      <c r="AR1" s="9" t="n">
+      <c r="AR1" s="12" t="n">
         <v>44713</v>
       </c>
-      <c r="AS1" s="9" t="n">
+      <c r="AS1" s="12" t="n">
         <v>44743</v>
       </c>
-      <c r="AT1" s="9" t="n">
+      <c r="AT1" s="12" t="n">
         <v>44774</v>
       </c>
-      <c r="AU1" s="9" t="n">
+      <c r="AU1" s="12" t="n">
         <v>44805</v>
       </c>
-      <c r="AV1" s="9" t="n">
+      <c r="AV1" s="12" t="n">
         <v>44835</v>
       </c>
-      <c r="AW1" s="9" t="n">
+      <c r="AW1" s="12" t="n">
         <v>44866</v>
       </c>
-      <c r="AX1" s="9" t="n">
+      <c r="AX1" s="12" t="n">
         <v>44896</v>
       </c>
-      <c r="AY1" s="9" t="n">
+      <c r="AY1" s="12" t="n">
         <v>44927</v>
       </c>
-      <c r="AZ1" s="9" t="n">
+      <c r="AZ1" s="12" t="n">
         <v>44958</v>
       </c>
-      <c r="BA1" s="9" t="n">
+      <c r="BA1" s="12" t="n">
         <v>44986</v>
       </c>
-      <c r="BB1" s="9" t="n">
+      <c r="BB1" s="12" t="n">
         <v>45017</v>
       </c>
-      <c r="BC1" s="9" t="n">
+      <c r="BC1" s="12" t="n">
         <v>45047</v>
       </c>
-      <c r="BD1" s="9" t="n">
+      <c r="BD1" s="12" t="n">
         <v>45078</v>
       </c>
-      <c r="BE1" s="9" t="n">
+      <c r="BE1" s="12" t="n">
         <v>45108</v>
       </c>
-      <c r="BF1" s="9" t="n">
+      <c r="BF1" s="12" t="n">
         <v>45139</v>
       </c>
-      <c r="BG1" s="9" t="n">
+      <c r="BG1" s="12" t="n">
         <v>45170</v>
       </c>
-      <c r="BH1" s="9" t="n">
+      <c r="BH1" s="12" t="n">
         <v>45200</v>
       </c>
-      <c r="BI1" s="9" t="n">
+      <c r="BI1" s="12" t="n">
         <v>45231</v>
       </c>
-      <c r="BJ1" s="9" t="n">
+      <c r="BJ1" s="12" t="n">
         <v>45261</v>
       </c>
-      <c r="BK1" s="9" t="n">
+      <c r="BK1" s="12" t="n">
         <v>45292</v>
       </c>
-      <c r="BL1" s="9" t="n">
+      <c r="BL1" s="12" t="n">
         <v>45323</v>
       </c>
-      <c r="BM1" s="9" t="n">
+      <c r="BM1" s="12" t="n">
         <v>45352</v>
       </c>
-      <c r="BN1" s="9" t="n">
+      <c r="BN1" s="12" t="n">
         <v>45383</v>
       </c>
-      <c r="BO1" s="9" t="n">
+      <c r="BO1" s="12" t="n">
         <v>45413</v>
       </c>
-      <c r="BP1" s="9" t="n">
+      <c r="BP1" s="12" t="n">
         <v>45444</v>
       </c>
-      <c r="BQ1" s="9" t="n">
+      <c r="BQ1" s="12" t="n">
         <v>45474</v>
       </c>
-      <c r="BR1" s="9" t="n">
+      <c r="BR1" s="12" t="n">
         <v>45505</v>
       </c>
-      <c r="BS1" s="9" t="n">
+      <c r="BS1" s="12" t="n">
         <v>45536</v>
       </c>
-      <c r="BT1" s="9" t="n">
+      <c r="BT1" s="12" t="n">
         <v>45566</v>
       </c>
-      <c r="BU1" s="9" t="n">
+      <c r="BU1" s="12" t="n">
         <v>45597</v>
       </c>
-      <c r="BV1" s="9" t="n">
+      <c r="BV1" s="12" t="n">
         <v>45627</v>
       </c>
-      <c r="BW1" s="9" t="n">
+      <c r="BW1" s="12" t="n">
         <v>45658</v>
       </c>
-      <c r="BX1" s="9" t="n">
+      <c r="BX1" s="12" t="n">
         <v>45689</v>
       </c>
-      <c r="BY1" s="9" t="n">
+      <c r="BY1" s="12" t="n">
         <v>45717</v>
       </c>
-      <c r="BZ1" s="9" t="n">
+      <c r="BZ1" s="12" t="n">
         <v>45748</v>
       </c>
-      <c r="CA1" s="9" t="n">
+      <c r="CA1" s="12" t="n">
         <v>45778</v>
       </c>
-      <c r="CB1" s="9" t="n">
+      <c r="CB1" s="12" t="n">
         <v>45809</v>
       </c>
-      <c r="CC1" s="9" t="n">
+      <c r="CC1" s="12" t="n">
         <v>45839</v>
       </c>
-      <c r="CD1" s="9" t="n">
+      <c r="CD1" s="12" t="n">
         <v>45870</v>
       </c>
-      <c r="CE1" s="9" t="n">
+      <c r="CE1" s="12" t="n">
         <v>45901</v>
       </c>
-      <c r="CF1" s="9" t="n">
+      <c r="CF1" s="12" t="n">
         <v>45931</v>
       </c>
-      <c r="CG1" s="9" t="n">
+      <c r="CG1" s="12" t="n">
         <v>45962</v>
       </c>
-      <c r="CH1" s="9" t="n">
+      <c r="CH1" s="12" t="n">
         <v>45992</v>
       </c>
     </row>

</xml_diff>